<commit_message>
testoversigt i TESTmappe opdateret
</commit_message>
<xml_diff>
--- a/Rapport/Test/TestOversigt.xlsx
+++ b/Rapport/Test/TestOversigt.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="18">
   <si>
     <t>Test id</t>
   </si>
@@ -31,13 +31,52 @@
   </si>
   <si>
     <t>Bestået</t>
+  </si>
+  <si>
+    <t>Søg på en eksisterende ordre</t>
+  </si>
+  <si>
+    <t>Anette</t>
+  </si>
+  <si>
+    <t>Søg på en ordre som ikke eksisterer</t>
+  </si>
+  <si>
+    <t>Søg på en eksisterende faktura</t>
+  </si>
+  <si>
+    <t>Søg på en faktura som ikke eksisterer</t>
+  </si>
+  <si>
+    <t>Test at systemet giver en fejlbesked når der indtastes bogstaver i søgefeltet</t>
+  </si>
+  <si>
+    <t>Opgrader en eksisterende ordre til en faktura</t>
+  </si>
+  <si>
+    <t>Opgrader en eksisterende ordre til en faktura og tilføj en bedemand.</t>
+  </si>
+  <si>
+    <t>Søg på en fakturanummer uden at tilføje "-" i fakturanummeret</t>
+  </si>
+  <si>
+    <t>Slet en eksisterende ordre</t>
+  </si>
+  <si>
+    <t>Slet en eksisterende faktura</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test at man kan oprette en ny bedemand </t>
+  </si>
+  <si>
+    <t>Ændre en faktura til at være betalt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,6 +91,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -86,7 +130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -95,6 +139,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -399,8 +447,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="75.140625" customWidth="1"/>
     <col min="3" max="3" width="25.140625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
@@ -420,103 +468,175 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="1">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="1">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="1">
-        <v>4</v>
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D5" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="1">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="1">
-        <v>6</v>
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="1">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="1">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="1">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
       <c r="C10" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D10" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="1">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
       <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D11" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="1">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
+      <c r="B12" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="C12" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D12" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="1">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
+      <c r="B13" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="C13" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="1">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -524,7 +644,7 @@
       </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="1">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -532,7 +652,7 @@
       </c>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="1">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -540,7 +660,7 @@
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="1">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -548,7 +668,7 @@
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="1">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -556,7 +676,7 @@
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="1">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -564,7 +684,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="1">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -572,7 +692,7 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="1">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -580,7 +700,7 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="1">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -588,7 +708,7 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="1">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -596,7 +716,7 @@
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="1">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -604,7 +724,7 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="1">
+      <c r="A25" s="5">
         <v>24</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -612,7 +732,7 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="1">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -620,7 +740,7 @@
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="1">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -628,7 +748,7 @@
       </c>
     </row>
     <row r="28" spans="1:3">
-      <c r="A28" s="1">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -636,7 +756,7 @@
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="1">
+      <c r="A29" s="5">
         <v>28</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -644,7 +764,7 @@
       </c>
     </row>
     <row r="30" spans="1:3">
-      <c r="A30" s="1">
+      <c r="A30" s="5">
         <v>29</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -652,7 +772,7 @@
       </c>
     </row>
     <row r="31" spans="1:3">
-      <c r="A31" s="1">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -660,7 +780,7 @@
       </c>
     </row>
     <row r="32" spans="1:3">
-      <c r="A32" s="1">
+      <c r="A32" s="5">
         <v>31</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -668,7 +788,7 @@
       </c>
     </row>
     <row r="33" spans="1:3">
-      <c r="A33" s="1">
+      <c r="A33" s="5">
         <v>32</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -676,7 +796,7 @@
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="1">
+      <c r="A34" s="5">
         <v>33</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -684,7 +804,7 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="1">
+      <c r="A35" s="5">
         <v>34</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -692,7 +812,7 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="1">
+      <c r="A36" s="5">
         <v>35</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -700,7 +820,7 @@
       </c>
     </row>
     <row r="37" spans="1:3">
-      <c r="A37" s="1">
+      <c r="A37" s="5">
         <v>36</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -708,7 +828,7 @@
       </c>
     </row>
     <row r="38" spans="1:3">
-      <c r="A38" s="1">
+      <c r="A38" s="5">
         <v>37</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -716,7 +836,7 @@
       </c>
     </row>
     <row r="39" spans="1:3">
-      <c r="A39" s="1">
+      <c r="A39" s="5">
         <v>38</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -724,7 +844,7 @@
       </c>
     </row>
     <row r="40" spans="1:3">
-      <c r="A40" s="1">
+      <c r="A40" s="5">
         <v>39</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -732,7 +852,7 @@
       </c>
     </row>
     <row r="41" spans="1:3">
-      <c r="A41" s="1">
+      <c r="A41" s="5">
         <v>40</v>
       </c>
       <c r="C41" s="3" t="s">

</xml_diff>

<commit_message>
Test på en hest
</commit_message>
<xml_diff>
--- a/Rapport/Test/TestOversigt.xlsx
+++ b/Rapport/Test/TestOversigt.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="19155" windowHeight="4680"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="54">
   <si>
     <t>Test id</t>
   </si>
@@ -175,12 +175,39 @@
       <t xml:space="preserve"> </t>
     </r>
   </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Log-in med forkert brugernavn</t>
+  </si>
+  <si>
+    <t>Start programmet med forkert database oplysninger</t>
+  </si>
+  <si>
+    <t>Opret en ordre og se om den trækker den rigtige moms</t>
+  </si>
+  <si>
+    <t>Thomas Af Danmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Søge på en bestemt varegruppe </t>
+  </si>
+  <si>
+    <t>Lager</t>
+  </si>
+  <si>
+    <t>Adminstration</t>
+  </si>
+  <si>
+    <t>Opret en pdf fil, der kan sendes til revisor.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,11 +305,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -310,6 +334,12 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -405,6 +435,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -439,6 +470,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kontor">
@@ -614,14 +646,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
     <col min="2" max="2" width="75.140625" customWidth="1"/>
@@ -629,583 +661,641 @@
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18.75">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="4">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="C12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="4"/>
-      <c r="B15" s="12" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="4">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>13</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="4">
+      <c r="C16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>14</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="4">
+      <c r="C17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>15</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="4">
+      <c r="C18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>16</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="4">
+      <c r="C19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
         <v>17</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="4">
+      <c r="C20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>18</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="4">
+      <c r="C21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>19</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="4">
+      <c r="C22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
         <v>20</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="4">
+      <c r="C23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
         <v>21</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="4">
+      <c r="C24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
         <v>22</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="4">
+      <c r="C25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
         <v>23</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="4">
+      <c r="C26" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
         <v>24</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="4">
+      <c r="C27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
         <v>25</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="4">
+      <c r="C28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
         <v>26</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="4">
+      <c r="C29" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
         <v>27</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="4">
+      <c r="C30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
         <v>28</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="4">
+      <c r="C31" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
         <v>29</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="4">
+      <c r="D32" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
         <v>30</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="4">
+      <c r="C33" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
         <v>31</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="4">
+      <c r="C34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
         <v>32</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="4">
+      <c r="C35" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
         <v>33</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="4">
+      <c r="C36" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
         <v>34</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>35</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="9" t="s">
+      <c r="C38" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="4"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="4">
-        <v>35</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="4">
+      <c r="D38" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
         <v>36</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D40" s="5"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="4">
+      <c r="B40" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
         <v>37</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" s="5"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="4">
+      <c r="B41" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="3"/>
+      <c r="B42" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="9"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
         <v>38</v>
       </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="5"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" s="4">
+      <c r="B43" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="9"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
         <v>39</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" s="5"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" s="4">
-        <v>40</v>
-      </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="1"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="1"/>
+      <c r="B45" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>40</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1214,24 +1304,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>